<commit_message>
range.Merge() won't call all cells in the range anymore. Fixed the way first/last cell works. They now take into account the row/column styles.
</commit_message>
<xml_diff>
--- a/ClosedXML/ClosedXML/ClosedXML_Tests/Resource/Examples/Misc/AdjustToContents.xlsx
+++ b/ClosedXML/ClosedXML/ClosedXML_Tests/Resource/Examples/Misc/AdjustToContents.xlsx
@@ -3495,7 +3495,7 @@
   <x:sheetPr>
     <x:outlinePr summaryBelow="1" summaryRight="1"/>
   </x:sheetPr>
-  <x:dimension ref="A1:D8"/>
+  <x:dimension ref="A1:B8"/>
   <x:sheetViews>
     <x:sheetView tabSelected="0" workbookViewId="0"/>
   </x:sheetViews>
@@ -3505,41 +3505,39 @@
     <x:col min="2" max="2" width="30.270625" style="0" customWidth="1"/>
   </x:cols>
   <x:sheetData>
-    <x:row r="1" spans="1:4" ht="41.65" customHeight="1">
+    <x:row r="1" spans="1:2" ht="41.65" customHeight="1">
       <x:c r="A1" s="1" t="s">
         <x:v>0</x:v>
       </x:c>
       <x:c r="B1" s="0" t="s"/>
     </x:row>
-    <x:row r="2" spans="1:4" ht="28.05" customHeight="1">
+    <x:row r="2" spans="1:2" ht="28.05" customHeight="1">
       <x:c r="A2" s="2" t="s">
         <x:v>1</x:v>
       </x:c>
       <x:c r="B2" s="0" t="s"/>
     </x:row>
-    <x:row r="4" spans="1:4">
+    <x:row r="4" spans="1:2">
       <x:c r="B4" s="0" t="s">
         <x:v>2</x:v>
       </x:c>
     </x:row>
-    <x:row r="5" spans="1:4">
+    <x:row r="5" spans="1:2">
       <x:c r="B5" s="0" t="s">
         <x:v>3</x:v>
       </x:c>
     </x:row>
-    <x:row r="6" spans="1:4">
+    <x:row r="6" spans="1:2">
       <x:c r="B6" s="0" t="s">
         <x:v>4</x:v>
       </x:c>
-      <x:c r="C6" s="0" t="s"/>
-      <x:c r="D6" s="0" t="s"/>
-    </x:row>
-    <x:row r="7" spans="1:4">
+    </x:row>
+    <x:row r="7" spans="1:2">
       <x:c r="B7" s="0" t="s">
         <x:v>5</x:v>
       </x:c>
     </x:row>
-    <x:row r="8" spans="1:4">
+    <x:row r="8" spans="1:2">
       <x:c r="B8" s="0" t="s">
         <x:v>2</x:v>
       </x:c>

</xml_diff>

<commit_message>
Fixed issue with row heights
</commit_message>
<xml_diff>
--- a/ClosedXML/ClosedXML/ClosedXML_Tests/Resource/Examples/Misc/AdjustToContents.xlsx
+++ b/ClosedXML/ClosedXML/ClosedXML_Tests/Resource/Examples/Misc/AdjustToContents.xlsx
@@ -3505,13 +3505,13 @@
     <x:col min="2" max="2" width="30.270625" style="0" customWidth="1"/>
   </x:cols>
   <x:sheetData>
-    <x:row r="1" spans="1:2" ht="41.65" customHeight="1">
+    <x:row r="1" spans="1:2" customFormat="1" ht="41.65" customHeight="1">
       <x:c r="A1" s="1" t="s">
         <x:v>0</x:v>
       </x:c>
       <x:c r="B1" s="0" t="s"/>
     </x:row>
-    <x:row r="2" spans="1:2" ht="28.05" customHeight="1">
+    <x:row r="2" spans="1:2" customFormat="1" ht="28.05" customHeight="1">
       <x:c r="A2" s="2" t="s">
         <x:v>1</x:v>
       </x:c>
@@ -3765,97 +3765,97 @@
   </x:sheetViews>
   <x:sheetFormatPr defaultRowHeight="15"/>
   <x:sheetData>
-    <x:row r="1" spans="1:1" ht="306" customHeight="1">
+    <x:row r="1" spans="1:1" customFormat="1" ht="306" customHeight="1">
       <x:c r="A1" s="3" t="s">
         <x:v>6</x:v>
       </x:c>
     </x:row>
-    <x:row r="2" spans="1:1" ht="15.299999999999999" customHeight="1">
+    <x:row r="2" spans="1:1" customFormat="1" ht="15.299999999999999" customHeight="1">
       <x:c r="A2" s="0" t="s">
         <x:v>7</x:v>
       </x:c>
     </x:row>
-    <x:row r="3" spans="1:1" ht="7.6499999999999986" customHeight="1">
+    <x:row r="3" spans="1:1" customFormat="1" ht="7.6499999999999986" customHeight="1">
       <x:c r="A3" s="4" t="s">
         <x:v>8</x:v>
       </x:c>
     </x:row>
-    <x:row r="4" spans="1:1" ht="16.15" customHeight="1">
+    <x:row r="4" spans="1:1" customFormat="1" ht="16.15" customHeight="1">
       <x:c r="A4" s="5" t="s">
         <x:v>9</x:v>
       </x:c>
     </x:row>
-    <x:row r="5" spans="1:1" ht="24.224999999999998" customHeight="1">
+    <x:row r="5" spans="1:1" customFormat="1" ht="24.224999999999998" customHeight="1">
       <x:c r="A5" s="6" t="s">
         <x:v>10</x:v>
       </x:c>
     </x:row>
-    <x:row r="6" spans="1:1" ht="32.3" customHeight="1">
+    <x:row r="6" spans="1:1" customFormat="1" ht="32.3" customHeight="1">
       <x:c r="A6" s="7" t="s">
         <x:v>11</x:v>
       </x:c>
     </x:row>
-    <x:row r="7" spans="1:1" ht="40.375" customHeight="1">
+    <x:row r="7" spans="1:1" customFormat="1" ht="40.375" customHeight="1">
       <x:c r="A7" s="8" t="s">
         <x:v>12</x:v>
       </x:c>
     </x:row>
-    <x:row r="8" spans="1:1" ht="48.449999999999996" customHeight="1">
+    <x:row r="8" spans="1:1" customFormat="1" ht="48.449999999999996" customHeight="1">
       <x:c r="A8" s="9" t="s">
         <x:v>13</x:v>
       </x:c>
     </x:row>
-    <x:row r="9" spans="1:1" ht="56.524999999999991" customHeight="1">
+    <x:row r="9" spans="1:1" customFormat="1" ht="56.524999999999991" customHeight="1">
       <x:c r="A9" s="10" t="s">
         <x:v>14</x:v>
       </x:c>
     </x:row>
-    <x:row r="10" spans="1:1" ht="64.6" customHeight="1">
+    <x:row r="10" spans="1:1" customFormat="1" ht="64.6" customHeight="1">
       <x:c r="A10" s="11" t="s">
         <x:v>15</x:v>
       </x:c>
     </x:row>
-    <x:row r="11" spans="1:1" ht="72.675" customHeight="1">
+    <x:row r="11" spans="1:1" customFormat="1" ht="72.675" customHeight="1">
       <x:c r="A11" s="12" t="s">
         <x:v>16</x:v>
       </x:c>
     </x:row>
-    <x:row r="12" spans="1:1" ht="80.75" customHeight="1">
+    <x:row r="12" spans="1:1" customFormat="1" ht="80.75" customHeight="1">
       <x:c r="A12" s="13" t="s">
         <x:v>17</x:v>
       </x:c>
     </x:row>
-    <x:row r="13" spans="1:1" ht="88.825" customHeight="1">
+    <x:row r="13" spans="1:1" customFormat="1" ht="88.825" customHeight="1">
       <x:c r="A13" s="14" t="s">
         <x:v>18</x:v>
       </x:c>
     </x:row>
-    <x:row r="14" spans="1:1" ht="96.899999999999991" customHeight="1">
+    <x:row r="14" spans="1:1" customFormat="1" ht="96.899999999999991" customHeight="1">
       <x:c r="A14" s="15" t="s">
         <x:v>19</x:v>
       </x:c>
     </x:row>
-    <x:row r="15" spans="1:1" ht="104.975" customHeight="1">
+    <x:row r="15" spans="1:1" customFormat="1" ht="104.975" customHeight="1">
       <x:c r="A15" s="16" t="s">
         <x:v>20</x:v>
       </x:c>
     </x:row>
-    <x:row r="16" spans="1:1" ht="113.04999999999998" customHeight="1">
+    <x:row r="16" spans="1:1" customFormat="1" ht="113.04999999999998" customHeight="1">
       <x:c r="A16" s="17" t="s">
         <x:v>21</x:v>
       </x:c>
     </x:row>
-    <x:row r="17" spans="1:1" ht="121.125" customHeight="1">
+    <x:row r="17" spans="1:1" customFormat="1" ht="121.125" customHeight="1">
       <x:c r="A17" s="18" t="s">
         <x:v>22</x:v>
       </x:c>
     </x:row>
-    <x:row r="18" spans="1:1" ht="129.2" customHeight="1">
+    <x:row r="18" spans="1:1" customFormat="1" ht="129.2" customHeight="1">
       <x:c r="A18" s="19" t="s">
         <x:v>23</x:v>
       </x:c>
     </x:row>
-    <x:row r="19" spans="1:1" ht="137.275" customHeight="1">
+    <x:row r="19" spans="1:1" customFormat="1" ht="137.275" customHeight="1">
       <x:c r="A19" s="20" t="s">
         <x:v>24</x:v>
       </x:c>
@@ -3880,97 +3880,97 @@
   </x:sheetViews>
   <x:sheetFormatPr defaultRowHeight="15"/>
   <x:sheetData>
-    <x:row r="1" spans="1:1" ht="306" customHeight="1">
+    <x:row r="1" spans="1:1" customFormat="1" ht="306" customHeight="1">
       <x:c r="A1" s="3" t="s">
         <x:v>6</x:v>
       </x:c>
     </x:row>
-    <x:row r="2" spans="1:1" ht="81.6" customHeight="1">
+    <x:row r="2" spans="1:1" customFormat="1" ht="81.6" customHeight="1">
       <x:c r="A2" s="0" t="s">
         <x:v>43</x:v>
       </x:c>
     </x:row>
-    <x:row r="3" spans="1:1" ht="16.999999999999996" customHeight="1">
+    <x:row r="3" spans="1:1" customFormat="1" ht="16.999999999999996" customHeight="1">
       <x:c r="A3" s="4" t="s">
         <x:v>44</x:v>
       </x:c>
     </x:row>
-    <x:row r="4" spans="1:1" ht="33.999999999999993" customHeight="1">
+    <x:row r="4" spans="1:1" customFormat="1" ht="33.999999999999993" customHeight="1">
       <x:c r="A4" s="5" t="s">
         <x:v>45</x:v>
       </x:c>
     </x:row>
-    <x:row r="5" spans="1:1" ht="50.999999999999993" customHeight="1">
+    <x:row r="5" spans="1:1" customFormat="1" ht="50.999999999999993" customHeight="1">
       <x:c r="A5" s="6" t="s">
         <x:v>46</x:v>
       </x:c>
     </x:row>
-    <x:row r="6" spans="1:1" ht="67.999999999999986" customHeight="1">
+    <x:row r="6" spans="1:1" customFormat="1" ht="67.999999999999986" customHeight="1">
       <x:c r="A6" s="7" t="s">
         <x:v>47</x:v>
       </x:c>
     </x:row>
-    <x:row r="7" spans="1:1" ht="85" customHeight="1">
+    <x:row r="7" spans="1:1" customFormat="1" ht="85" customHeight="1">
       <x:c r="A7" s="8" t="s">
         <x:v>48</x:v>
       </x:c>
     </x:row>
-    <x:row r="8" spans="1:1" ht="101.99999999999999" customHeight="1">
+    <x:row r="8" spans="1:1" customFormat="1" ht="101.99999999999999" customHeight="1">
       <x:c r="A8" s="9" t="s">
         <x:v>49</x:v>
       </x:c>
     </x:row>
-    <x:row r="9" spans="1:1" ht="118.99999999999999" customHeight="1">
+    <x:row r="9" spans="1:1" customFormat="1" ht="118.99999999999999" customHeight="1">
       <x:c r="A9" s="10" t="s">
         <x:v>50</x:v>
       </x:c>
     </x:row>
-    <x:row r="10" spans="1:1" ht="135.99999999999997" customHeight="1">
+    <x:row r="10" spans="1:1" customFormat="1" ht="135.99999999999997" customHeight="1">
       <x:c r="A10" s="11" t="s">
         <x:v>51</x:v>
       </x:c>
     </x:row>
-    <x:row r="11" spans="1:1" ht="153" customHeight="1">
+    <x:row r="11" spans="1:1" customFormat="1" ht="153" customHeight="1">
       <x:c r="A11" s="12" t="s">
         <x:v>52</x:v>
       </x:c>
     </x:row>
-    <x:row r="12" spans="1:1" ht="170" customHeight="1">
+    <x:row r="12" spans="1:1" customFormat="1" ht="170" customHeight="1">
       <x:c r="A12" s="13" t="s">
         <x:v>53</x:v>
       </x:c>
     </x:row>
-    <x:row r="13" spans="1:1" ht="187" customHeight="1">
+    <x:row r="13" spans="1:1" customFormat="1" ht="187" customHeight="1">
       <x:c r="A13" s="14" t="s">
         <x:v>54</x:v>
       </x:c>
     </x:row>
-    <x:row r="14" spans="1:1" ht="203.99999999999997" customHeight="1">
+    <x:row r="14" spans="1:1" customFormat="1" ht="203.99999999999997" customHeight="1">
       <x:c r="A14" s="15" t="s">
         <x:v>55</x:v>
       </x:c>
     </x:row>
-    <x:row r="15" spans="1:1" ht="221" customHeight="1">
+    <x:row r="15" spans="1:1" customFormat="1" ht="221" customHeight="1">
       <x:c r="A15" s="16" t="s">
         <x:v>56</x:v>
       </x:c>
     </x:row>
-    <x:row r="16" spans="1:1" ht="237.99999999999997" customHeight="1">
+    <x:row r="16" spans="1:1" customFormat="1" ht="237.99999999999997" customHeight="1">
       <x:c r="A16" s="17" t="s">
         <x:v>57</x:v>
       </x:c>
     </x:row>
-    <x:row r="17" spans="1:1" ht="255" customHeight="1">
+    <x:row r="17" spans="1:1" customFormat="1" ht="255" customHeight="1">
       <x:c r="A17" s="18" t="s">
         <x:v>58</x:v>
       </x:c>
     </x:row>
-    <x:row r="18" spans="1:1" ht="271.99999999999994" customHeight="1">
+    <x:row r="18" spans="1:1" customFormat="1" ht="271.99999999999994" customHeight="1">
       <x:c r="A18" s="19" t="s">
         <x:v>59</x:v>
       </x:c>
     </x:row>
-    <x:row r="19" spans="1:1" ht="289" customHeight="1">
+    <x:row r="19" spans="1:1" customFormat="1" ht="289" customHeight="1">
       <x:c r="A19" s="20" t="s">
         <x:v>60</x:v>
       </x:c>

</xml_diff>

<commit_message>
Update Adjust to contents (gotta love doubles)
</commit_message>
<xml_diff>
--- a/ClosedXML/ClosedXML/ClosedXML_Tests/Resource/Examples/Misc/AdjustToContents.xlsx
+++ b/ClosedXML/ClosedXML/ClosedXML_Tests/Resource/Examples/Misc/AdjustToContents.xlsx
@@ -3575,14 +3575,14 @@
     <x:col min="1" max="1" width="2.9306249999999996" style="0" customWidth="1"/>
     <x:col min="2" max="2" width="16.150624999999998" style="0" customWidth="1"/>
     <x:col min="3" max="3" width="17.315676440444804" style="0" customWidth="1"/>
-    <x:col min="4" max="4" width="18.195145171689223" style="0" customWidth="1"/>
+    <x:col min="4" max="4" width="18.195145171689227" style="0" customWidth="1"/>
     <x:col min="5" max="5" width="17.902475307480557" style="0" customWidth="1"/>
     <x:col min="6" max="6" width="17.495860622181581" style="0" customWidth="1"/>
     <x:col min="7" max="7" width="16.978395699068074" style="0" customWidth="1"/>
     <x:col min="8" max="8" width="16.3540187586588" style="0" customWidth="1"/>
     <x:col min="9" max="9" width="15.627481686479374" style="0" customWidth="1"/>
-    <x:col min="10" max="10" width="14.80431386834416" style="0" customWidth="1"/>
-    <x:col min="11" max="11" width="13.890780108391489" style="0" customWidth="1"/>
+    <x:col min="10" max="10" width="14.804313868344162" style="0" customWidth="1"/>
+    <x:col min="11" max="11" width="13.890780108391487" style="0" customWidth="1"/>
     <x:col min="12" max="12" width="12.893832950141361" style="0" customWidth="1"/>
     <x:col min="13" max="13" width="11.821059763441216" style="0" customWidth="1"/>
     <x:col min="14" max="14" width="10.680625000000003" style="0" customWidth="1"/>
@@ -3674,18 +3674,18 @@
   <x:cols>
     <x:col min="1" max="1" width="2.9306249999999996" style="0" customWidth="1"/>
     <x:col min="2" max="2" width="51.020625" style="0" customWidth="1"/>
-    <x:col min="3" max="3" width="61.832985562903978" style="0" customWidth="1"/>
+    <x:col min="3" max="3" width="61.832985562903971" style="0" customWidth="1"/>
     <x:col min="4" max="4" width="61.271495301031983" style="0" customWidth="1"/>
-    <x:col min="5" max="5" width="60.340427494313964" style="0" customWidth="1"/>
-    <x:col min="6" max="6" width="59.04686813095315" style="0" customWidth="1"/>
-    <x:col min="7" max="7" width="57.400661978777208" style="0" customWidth="1"/>
-    <x:col min="8" max="8" width="55.414337660610677" style="0" customWidth="1"/>
+    <x:col min="5" max="5" width="60.340427494313957" style="0" customWidth="1"/>
+    <x:col min="6" max="6" width="59.046868130953143" style="0" customWidth="1"/>
+    <x:col min="7" max="7" width="57.400661978777215" style="0" customWidth="1"/>
+    <x:col min="8" max="8" width="55.41433766061067" style="0" customWidth="1"/>
     <x:col min="9" max="9" width="53.103012303890189" style="0" customWidth="1"/>
-    <x:col min="10" max="10" width="50.484276490196805" style="0" customWidth="1"/>
+    <x:col min="10" max="10" width="50.484276490196812" style="0" customWidth="1"/>
     <x:col min="11" max="11" width="47.578060380308663" style="0" customWidth="1"/>
     <x:col min="12" max="12" width="44.406482033643258" style="0" customWidth="1"/>
-    <x:col min="13" max="13" width="40.993679076470087" style="0" customWidth="1"/>
-    <x:col min="14" max="14" width="37.365625000000009" style="0" customWidth="1"/>
+    <x:col min="13" max="13" width="40.99367907647008" style="0" customWidth="1"/>
+    <x:col min="14" max="14" width="37.365625" style="0" customWidth="1"/>
     <x:col min="15" max="15" width="33.549931486433891" style="0" customWidth="1"/>
     <x:col min="16" max="16" width="29.575638267388729" style="0" customWidth="1"/>
     <x:col min="17" max="17" width="25.4729921140053" style="0" customWidth="1"/>

</xml_diff>